<commit_message>
results as of 02/08/18
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="274">
   <si>
     <t>Date</t>
   </si>
@@ -828,6 +828,15 @@
   </si>
   <si>
     <t>17:46</t>
+  </si>
+  <si>
+    <t>Jul-31</t>
+  </si>
+  <si>
+    <t>Aug-01</t>
+  </si>
+  <si>
+    <t>Aug-02</t>
   </si>
 </sst>
 </file>
@@ -1246,7 +1255,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G269"/>
+  <dimension ref="A1:G402"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="E27" activeCellId="0" pane="topLeft" sqref="E27"/>
@@ -6951,6 +6960,2267 @@
       </c>
       <c r="E269" t="n">
         <v>26.78</v>
+      </c>
+    </row>
+    <row r="270" spans="1:7">
+      <c r="A270" t="s">
+        <v>230</v>
+      </c>
+      <c r="B270" t="s">
+        <v>42</v>
+      </c>
+      <c r="C270" t="n">
+        <v>9.949999999999999</v>
+      </c>
+      <c r="D270" t="n">
+        <v>3.17</v>
+      </c>
+      <c r="E270" t="n">
+        <v>32.33</v>
+      </c>
+    </row>
+    <row r="271" spans="1:7">
+      <c r="A271" t="s">
+        <v>230</v>
+      </c>
+      <c r="B271" t="s">
+        <v>43</v>
+      </c>
+      <c r="C271" t="n">
+        <v>8.279999999999999</v>
+      </c>
+      <c r="D271" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="E271" t="n">
+        <v>51.32</v>
+      </c>
+    </row>
+    <row r="272" spans="1:7">
+      <c r="A272" t="s">
+        <v>230</v>
+      </c>
+      <c r="B272" t="s">
+        <v>44</v>
+      </c>
+      <c r="C272" t="n">
+        <v>9.380000000000001</v>
+      </c>
+      <c r="D272" t="n">
+        <v>2.03</v>
+      </c>
+      <c r="E272" t="n">
+        <v>31.01</v>
+      </c>
+    </row>
+    <row r="273" spans="1:7">
+      <c r="A273" t="s">
+        <v>230</v>
+      </c>
+      <c r="B273" t="s">
+        <v>45</v>
+      </c>
+      <c r="C273" t="n">
+        <v>9.9</v>
+      </c>
+      <c r="D273" t="n">
+        <v>2.36</v>
+      </c>
+      <c r="E273" t="n">
+        <v>36.43</v>
+      </c>
+    </row>
+    <row r="274" spans="1:7">
+      <c r="A274" t="s">
+        <v>230</v>
+      </c>
+      <c r="B274" t="s">
+        <v>46</v>
+      </c>
+      <c r="C274" t="n">
+        <v>9.98</v>
+      </c>
+      <c r="D274" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="E274" t="n">
+        <v>28.55</v>
+      </c>
+    </row>
+    <row r="275" spans="1:7">
+      <c r="A275" t="s">
+        <v>230</v>
+      </c>
+      <c r="B275" t="s">
+        <v>47</v>
+      </c>
+      <c r="C275" t="n">
+        <v>8.99</v>
+      </c>
+      <c r="D275" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="E275" t="n">
+        <v>50.61</v>
+      </c>
+    </row>
+    <row r="276" spans="1:7">
+      <c r="A276" t="s">
+        <v>230</v>
+      </c>
+      <c r="B276" t="s">
+        <v>48</v>
+      </c>
+      <c r="C276" t="n">
+        <v>10.28</v>
+      </c>
+      <c r="D276" t="n">
+        <v>1.81</v>
+      </c>
+      <c r="E276" t="n">
+        <v>31.84</v>
+      </c>
+    </row>
+    <row r="277" spans="1:7">
+      <c r="A277" t="s">
+        <v>230</v>
+      </c>
+      <c r="B277" t="s">
+        <v>31</v>
+      </c>
+      <c r="C277" t="n">
+        <v>10.02</v>
+      </c>
+      <c r="D277" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="E277" t="n">
+        <v>54.66</v>
+      </c>
+    </row>
+    <row r="278" spans="1:7">
+      <c r="A278" t="s">
+        <v>230</v>
+      </c>
+      <c r="B278" t="s">
+        <v>32</v>
+      </c>
+      <c r="C278" t="n">
+        <v>10.29</v>
+      </c>
+      <c r="D278" t="n">
+        <v>1.76</v>
+      </c>
+      <c r="E278" t="n">
+        <v>28.33</v>
+      </c>
+    </row>
+    <row r="279" spans="1:7">
+      <c r="A279" t="s">
+        <v>230</v>
+      </c>
+      <c r="B279" t="s">
+        <v>33</v>
+      </c>
+      <c r="C279" t="n">
+        <v>8.369999999999999</v>
+      </c>
+      <c r="D279" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="E279" t="n">
+        <v>61.51</v>
+      </c>
+    </row>
+    <row r="280" spans="1:7">
+      <c r="A280" t="s">
+        <v>230</v>
+      </c>
+      <c r="B280" t="s">
+        <v>34</v>
+      </c>
+      <c r="C280" t="n">
+        <v>8.74</v>
+      </c>
+      <c r="D280" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="E280" t="n">
+        <v>57.34</v>
+      </c>
+    </row>
+    <row r="281" spans="1:7">
+      <c r="A281" t="s">
+        <v>230</v>
+      </c>
+      <c r="B281" t="s">
+        <v>35</v>
+      </c>
+      <c r="C281" t="n">
+        <v>9.9</v>
+      </c>
+      <c r="D281" t="n">
+        <v>1.96</v>
+      </c>
+      <c r="E281" t="n">
+        <v>42.36</v>
+      </c>
+    </row>
+    <row r="282" spans="1:7">
+      <c r="A282" t="s">
+        <v>271</v>
+      </c>
+      <c r="B282" t="s">
+        <v>50</v>
+      </c>
+      <c r="C282" t="n">
+        <v>9.199999999999999</v>
+      </c>
+      <c r="D282" t="n">
+        <v>2.07</v>
+      </c>
+      <c r="E282" t="n">
+        <v>39.52</v>
+      </c>
+    </row>
+    <row r="283" spans="1:7">
+      <c r="A283" t="s">
+        <v>271</v>
+      </c>
+      <c r="B283" t="s">
+        <v>51</v>
+      </c>
+      <c r="C283" t="n">
+        <v>9.51</v>
+      </c>
+      <c r="D283" t="n">
+        <v>2.07</v>
+      </c>
+      <c r="E283" t="n">
+        <v>54.05</v>
+      </c>
+    </row>
+    <row r="284" spans="1:7">
+      <c r="A284" t="s">
+        <v>271</v>
+      </c>
+      <c r="B284" t="s">
+        <v>37</v>
+      </c>
+      <c r="C284" t="n">
+        <v>10.39</v>
+      </c>
+      <c r="D284" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="E284" t="n">
+        <v>28.88</v>
+      </c>
+    </row>
+    <row r="285" spans="1:7">
+      <c r="A285" t="s">
+        <v>271</v>
+      </c>
+      <c r="B285" t="s">
+        <v>38</v>
+      </c>
+      <c r="C285" t="n">
+        <v>10.43</v>
+      </c>
+      <c r="D285" t="n">
+        <v>8.789999999999999</v>
+      </c>
+      <c r="E285" t="n">
+        <v>32.77</v>
+      </c>
+    </row>
+    <row r="286" spans="1:7">
+      <c r="A286" t="s">
+        <v>271</v>
+      </c>
+      <c r="B286" t="s">
+        <v>52</v>
+      </c>
+      <c r="C286" t="n">
+        <v>10.36</v>
+      </c>
+      <c r="D286" t="n">
+        <v>9.140000000000001</v>
+      </c>
+      <c r="E286" t="n">
+        <v>25.53</v>
+      </c>
+    </row>
+    <row r="287" spans="1:7">
+      <c r="A287" t="s">
+        <v>271</v>
+      </c>
+      <c r="B287" t="s">
+        <v>53</v>
+      </c>
+      <c r="C287" t="n">
+        <v>10.35</v>
+      </c>
+      <c r="D287" t="n">
+        <v>8.59</v>
+      </c>
+      <c r="E287" t="n">
+        <v>33.03</v>
+      </c>
+    </row>
+    <row r="288" spans="1:7">
+      <c r="A288" t="s">
+        <v>271</v>
+      </c>
+      <c r="B288" t="s">
+        <v>54</v>
+      </c>
+      <c r="C288" t="n">
+        <v>10.36</v>
+      </c>
+      <c r="D288" t="n">
+        <v>8.92</v>
+      </c>
+      <c r="E288" t="n">
+        <v>36.69</v>
+      </c>
+    </row>
+    <row r="289" spans="1:7">
+      <c r="A289" t="s">
+        <v>271</v>
+      </c>
+      <c r="B289" t="s">
+        <v>55</v>
+      </c>
+      <c r="C289" t="n">
+        <v>9.98</v>
+      </c>
+      <c r="D289" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="E289" t="n">
+        <v>25.96</v>
+      </c>
+    </row>
+    <row r="290" spans="1:7">
+      <c r="A290" t="s">
+        <v>271</v>
+      </c>
+      <c r="B290" t="s">
+        <v>56</v>
+      </c>
+      <c r="C290" t="n">
+        <v>10.36</v>
+      </c>
+      <c r="D290" t="n">
+        <v>10.17</v>
+      </c>
+      <c r="E290" t="n">
+        <v>25.59</v>
+      </c>
+    </row>
+    <row r="291" spans="1:7">
+      <c r="A291" t="s">
+        <v>271</v>
+      </c>
+      <c r="B291" t="s">
+        <v>57</v>
+      </c>
+      <c r="C291" t="n">
+        <v>10.36</v>
+      </c>
+      <c r="D291" t="n">
+        <v>10.02</v>
+      </c>
+      <c r="E291" t="n">
+        <v>26.08</v>
+      </c>
+    </row>
+    <row r="292" spans="1:7">
+      <c r="A292" t="s">
+        <v>271</v>
+      </c>
+      <c r="B292" t="s">
+        <v>58</v>
+      </c>
+      <c r="C292" t="n">
+        <v>9.75</v>
+      </c>
+      <c r="D292" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="E292" t="n">
+        <v>29.85</v>
+      </c>
+    </row>
+    <row r="293" spans="1:7">
+      <c r="A293" t="s">
+        <v>271</v>
+      </c>
+      <c r="B293" t="s">
+        <v>59</v>
+      </c>
+      <c r="C293" t="n">
+        <v>10.34</v>
+      </c>
+      <c r="D293" t="n">
+        <v>10.33</v>
+      </c>
+      <c r="E293" t="n">
+        <v>27.67</v>
+      </c>
+    </row>
+    <row r="294" spans="1:7">
+      <c r="A294" t="s">
+        <v>271</v>
+      </c>
+      <c r="B294" t="s">
+        <v>60</v>
+      </c>
+      <c r="C294" t="n">
+        <v>10.37</v>
+      </c>
+      <c r="D294" t="n">
+        <v>10.69</v>
+      </c>
+      <c r="E294" t="n">
+        <v>27.61</v>
+      </c>
+    </row>
+    <row r="295" spans="1:7">
+      <c r="A295" t="s">
+        <v>271</v>
+      </c>
+      <c r="B295" t="s">
+        <v>61</v>
+      </c>
+      <c r="C295" t="n">
+        <v>10.34</v>
+      </c>
+      <c r="D295" t="n">
+        <v>10.58</v>
+      </c>
+      <c r="E295" t="n">
+        <v>30.6</v>
+      </c>
+    </row>
+    <row r="296" spans="1:7">
+      <c r="A296" t="s">
+        <v>271</v>
+      </c>
+      <c r="B296" t="s">
+        <v>62</v>
+      </c>
+      <c r="C296" t="n">
+        <v>9.779999999999999</v>
+      </c>
+      <c r="D296" t="n">
+        <v>10.09</v>
+      </c>
+      <c r="E296" t="n">
+        <v>24.72</v>
+      </c>
+    </row>
+    <row r="297" spans="1:7">
+      <c r="A297" t="s">
+        <v>271</v>
+      </c>
+      <c r="B297" t="s">
+        <v>63</v>
+      </c>
+      <c r="C297" t="n">
+        <v>10</v>
+      </c>
+      <c r="D297" t="n">
+        <v>9.15</v>
+      </c>
+      <c r="E297" t="n">
+        <v>31.45</v>
+      </c>
+    </row>
+    <row r="298" spans="1:7">
+      <c r="A298" t="s">
+        <v>271</v>
+      </c>
+      <c r="B298" t="s">
+        <v>64</v>
+      </c>
+      <c r="C298" t="n">
+        <v>9.48</v>
+      </c>
+      <c r="D298" t="n">
+        <v>9</v>
+      </c>
+      <c r="E298" t="n">
+        <v>25.46</v>
+      </c>
+    </row>
+    <row r="299" spans="1:7">
+      <c r="A299" t="s">
+        <v>271</v>
+      </c>
+      <c r="B299" t="s">
+        <v>65</v>
+      </c>
+      <c r="C299" t="n">
+        <v>10.36</v>
+      </c>
+      <c r="D299" t="n">
+        <v>6.02</v>
+      </c>
+      <c r="E299" t="n">
+        <v>34.85</v>
+      </c>
+    </row>
+    <row r="300" spans="1:7">
+      <c r="A300" t="s">
+        <v>271</v>
+      </c>
+      <c r="B300" t="s">
+        <v>66</v>
+      </c>
+      <c r="C300" t="n">
+        <v>10.35</v>
+      </c>
+      <c r="D300" t="n">
+        <v>6.84</v>
+      </c>
+      <c r="E300" t="n">
+        <v>25.93</v>
+      </c>
+    </row>
+    <row r="301" spans="1:7">
+      <c r="A301" t="s">
+        <v>271</v>
+      </c>
+      <c r="B301" t="s">
+        <v>67</v>
+      </c>
+      <c r="C301" t="n">
+        <v>10.42</v>
+      </c>
+      <c r="D301" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="E301" t="n">
+        <v>29.79</v>
+      </c>
+    </row>
+    <row r="302" spans="1:7">
+      <c r="A302" t="s">
+        <v>271</v>
+      </c>
+      <c r="B302" t="s">
+        <v>68</v>
+      </c>
+      <c r="C302" t="n">
+        <v>10.28</v>
+      </c>
+      <c r="D302" t="n">
+        <v>3.46</v>
+      </c>
+      <c r="E302" t="n">
+        <v>26.34</v>
+      </c>
+    </row>
+    <row r="303" spans="1:7">
+      <c r="A303" t="s">
+        <v>271</v>
+      </c>
+      <c r="B303" t="s">
+        <v>69</v>
+      </c>
+      <c r="C303" t="n">
+        <v>10.06</v>
+      </c>
+      <c r="D303" t="n">
+        <v>4.77</v>
+      </c>
+      <c r="E303" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="304" spans="1:7">
+      <c r="A304" t="s">
+        <v>271</v>
+      </c>
+      <c r="B304" t="s">
+        <v>70</v>
+      </c>
+      <c r="C304" t="n">
+        <v>10.3</v>
+      </c>
+      <c r="D304" t="n">
+        <v>5.74</v>
+      </c>
+      <c r="E304" t="n">
+        <v>27.16</v>
+      </c>
+    </row>
+    <row r="305" spans="1:7">
+      <c r="A305" t="s">
+        <v>271</v>
+      </c>
+      <c r="B305" t="s">
+        <v>71</v>
+      </c>
+      <c r="C305" t="n">
+        <v>9.789999999999999</v>
+      </c>
+      <c r="D305" t="n">
+        <v>4.22</v>
+      </c>
+      <c r="E305" t="n">
+        <v>29.83</v>
+      </c>
+    </row>
+    <row r="306" spans="1:7">
+      <c r="A306" t="s">
+        <v>271</v>
+      </c>
+      <c r="B306" t="s">
+        <v>72</v>
+      </c>
+      <c r="C306" t="n">
+        <v>8.42</v>
+      </c>
+      <c r="D306" t="n">
+        <v>6.62</v>
+      </c>
+      <c r="E306" t="n">
+        <v>29.73</v>
+      </c>
+    </row>
+    <row r="307" spans="1:7">
+      <c r="A307" t="s">
+        <v>271</v>
+      </c>
+      <c r="B307" t="s">
+        <v>73</v>
+      </c>
+      <c r="C307" t="n">
+        <v>9.619999999999999</v>
+      </c>
+      <c r="D307" t="n">
+        <v>3.67</v>
+      </c>
+      <c r="E307" t="n">
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="308" spans="1:7">
+      <c r="A308" t="s">
+        <v>271</v>
+      </c>
+      <c r="B308" t="s">
+        <v>74</v>
+      </c>
+      <c r="C308" t="n">
+        <v>7.73</v>
+      </c>
+      <c r="D308" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="E308" t="n">
+        <v>35.84</v>
+      </c>
+    </row>
+    <row r="309" spans="1:7">
+      <c r="A309" t="s">
+        <v>271</v>
+      </c>
+      <c r="B309" t="s">
+        <v>111</v>
+      </c>
+      <c r="C309" t="n">
+        <v>9.82</v>
+      </c>
+      <c r="D309" t="n">
+        <v>2.21</v>
+      </c>
+      <c r="E309" t="n">
+        <v>32.44</v>
+      </c>
+    </row>
+    <row r="310" spans="1:7">
+      <c r="A310" t="s">
+        <v>271</v>
+      </c>
+      <c r="B310" t="s">
+        <v>113</v>
+      </c>
+      <c r="C310" t="n">
+        <v>9.84</v>
+      </c>
+      <c r="D310" t="n">
+        <v>2.96</v>
+      </c>
+      <c r="E310" t="n">
+        <v>29.28</v>
+      </c>
+    </row>
+    <row r="311" spans="1:7">
+      <c r="A311" t="s">
+        <v>271</v>
+      </c>
+      <c r="B311" t="s">
+        <v>39</v>
+      </c>
+      <c r="C311" t="n">
+        <v>10.14</v>
+      </c>
+      <c r="D311" t="n">
+        <v>3.81</v>
+      </c>
+      <c r="E311" t="n">
+        <v>34.07</v>
+      </c>
+    </row>
+    <row r="312" spans="1:7">
+      <c r="A312" t="s">
+        <v>271</v>
+      </c>
+      <c r="B312" t="s">
+        <v>40</v>
+      </c>
+      <c r="C312" t="n">
+        <v>9.58</v>
+      </c>
+      <c r="D312" t="n">
+        <v>3.61</v>
+      </c>
+      <c r="E312" t="n">
+        <v>36.26</v>
+      </c>
+    </row>
+    <row r="313" spans="1:7">
+      <c r="A313" t="s">
+        <v>271</v>
+      </c>
+      <c r="B313" t="s">
+        <v>11</v>
+      </c>
+      <c r="C313" t="n">
+        <v>10.17</v>
+      </c>
+      <c r="D313" t="n">
+        <v>2.74</v>
+      </c>
+      <c r="E313" t="n">
+        <v>32.88</v>
+      </c>
+    </row>
+    <row r="314" spans="1:7">
+      <c r="A314" t="s">
+        <v>271</v>
+      </c>
+      <c r="B314" t="s">
+        <v>17</v>
+      </c>
+      <c r="C314" t="n">
+        <v>10.17</v>
+      </c>
+      <c r="D314" t="n">
+        <v>3.81</v>
+      </c>
+      <c r="E314" t="n">
+        <v>34.05</v>
+      </c>
+    </row>
+    <row r="315" spans="1:7">
+      <c r="A315" t="s">
+        <v>271</v>
+      </c>
+      <c r="B315" t="s">
+        <v>23</v>
+      </c>
+      <c r="C315" t="n">
+        <v>5.63</v>
+      </c>
+      <c r="D315" t="n">
+        <v>1.44</v>
+      </c>
+      <c r="E315" t="n">
+        <v>54.38</v>
+      </c>
+    </row>
+    <row r="316" spans="1:7">
+      <c r="A316" t="s">
+        <v>271</v>
+      </c>
+      <c r="B316" t="s">
+        <v>28</v>
+      </c>
+      <c r="C316" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="D316" t="n">
+        <v>4.34</v>
+      </c>
+      <c r="E316" t="n">
+        <v>34.4</v>
+      </c>
+    </row>
+    <row r="317" spans="1:7">
+      <c r="A317" t="s">
+        <v>271</v>
+      </c>
+      <c r="B317" t="s">
+        <v>41</v>
+      </c>
+      <c r="C317" t="n">
+        <v>10.14</v>
+      </c>
+      <c r="D317" t="n">
+        <v>1.88</v>
+      </c>
+      <c r="E317" t="n">
+        <v>31.05</v>
+      </c>
+    </row>
+    <row r="318" spans="1:7">
+      <c r="A318" t="s">
+        <v>271</v>
+      </c>
+      <c r="B318" t="s">
+        <v>42</v>
+      </c>
+      <c r="C318" t="n">
+        <v>6.84</v>
+      </c>
+      <c r="D318" t="n">
+        <v>2.13</v>
+      </c>
+      <c r="E318" t="n">
+        <v>43.39</v>
+      </c>
+    </row>
+    <row r="319" spans="1:7">
+      <c r="A319" t="s">
+        <v>271</v>
+      </c>
+      <c r="B319" t="s">
+        <v>43</v>
+      </c>
+      <c r="C319" t="n">
+        <v>5.17</v>
+      </c>
+      <c r="D319" t="n">
+        <v>2.04</v>
+      </c>
+      <c r="E319" t="n">
+        <v>100.13</v>
+      </c>
+    </row>
+    <row r="320" spans="1:7">
+      <c r="A320" t="s">
+        <v>271</v>
+      </c>
+      <c r="B320" t="s">
+        <v>44</v>
+      </c>
+      <c r="C320" t="n">
+        <v>7.43</v>
+      </c>
+      <c r="D320" t="n">
+        <v>2.28</v>
+      </c>
+      <c r="E320" t="n">
+        <v>44.67</v>
+      </c>
+    </row>
+    <row r="321" spans="1:7">
+      <c r="A321" t="s">
+        <v>271</v>
+      </c>
+      <c r="B321" t="s">
+        <v>45</v>
+      </c>
+      <c r="C321" t="n">
+        <v>10.13</v>
+      </c>
+      <c r="D321" t="n">
+        <v>2.19</v>
+      </c>
+      <c r="E321" t="n">
+        <v>31.09</v>
+      </c>
+    </row>
+    <row r="322" spans="1:7">
+      <c r="A322" t="s">
+        <v>271</v>
+      </c>
+      <c r="B322" t="s">
+        <v>46</v>
+      </c>
+      <c r="C322" t="n">
+        <v>9.67</v>
+      </c>
+      <c r="D322" t="n">
+        <v>4.07</v>
+      </c>
+      <c r="E322" t="n">
+        <v>27.15</v>
+      </c>
+    </row>
+    <row r="323" spans="1:7">
+      <c r="A323" t="s">
+        <v>271</v>
+      </c>
+      <c r="B323" t="s">
+        <v>47</v>
+      </c>
+      <c r="C323" t="n">
+        <v>9.41</v>
+      </c>
+      <c r="D323" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="E323" t="n">
+        <v>38.62</v>
+      </c>
+    </row>
+    <row r="324" spans="1:7">
+      <c r="A324" t="s">
+        <v>271</v>
+      </c>
+      <c r="B324" t="s">
+        <v>48</v>
+      </c>
+      <c r="C324" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D324" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="E324" t="n">
+        <v>38.78</v>
+      </c>
+    </row>
+    <row r="325" spans="1:7">
+      <c r="A325" t="s">
+        <v>271</v>
+      </c>
+      <c r="B325" t="s">
+        <v>31</v>
+      </c>
+      <c r="C325" t="n">
+        <v>10.04</v>
+      </c>
+      <c r="D325" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="E325" t="n">
+        <v>37.06</v>
+      </c>
+    </row>
+    <row r="326" spans="1:7">
+      <c r="A326" t="s">
+        <v>271</v>
+      </c>
+      <c r="B326" t="s">
+        <v>32</v>
+      </c>
+      <c r="C326" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="D326" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E326" t="n">
+        <v>53.32</v>
+      </c>
+    </row>
+    <row r="327" spans="1:7">
+      <c r="A327" t="s">
+        <v>271</v>
+      </c>
+      <c r="B327" t="s">
+        <v>33</v>
+      </c>
+      <c r="C327" t="n">
+        <v>5.14</v>
+      </c>
+      <c r="D327" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="E327" t="n">
+        <v>55.2</v>
+      </c>
+    </row>
+    <row r="328" spans="1:7">
+      <c r="A328" t="s">
+        <v>271</v>
+      </c>
+      <c r="B328" t="s">
+        <v>34</v>
+      </c>
+      <c r="C328" t="n">
+        <v>9.06</v>
+      </c>
+      <c r="D328" t="n">
+        <v>1.16</v>
+      </c>
+      <c r="E328" t="n">
+        <v>42.37</v>
+      </c>
+    </row>
+    <row r="329" spans="1:7">
+      <c r="A329" t="s">
+        <v>271</v>
+      </c>
+      <c r="B329" t="s">
+        <v>35</v>
+      </c>
+      <c r="C329" t="n">
+        <v>2.76</v>
+      </c>
+      <c r="D329" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="E329" t="n">
+        <v>97.04000000000001</v>
+      </c>
+    </row>
+    <row r="330" spans="1:7">
+      <c r="A330" t="s">
+        <v>272</v>
+      </c>
+      <c r="B330" t="s">
+        <v>50</v>
+      </c>
+      <c r="C330" t="n">
+        <v>9.83</v>
+      </c>
+      <c r="D330" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="E330" t="n">
+        <v>33.9</v>
+      </c>
+    </row>
+    <row r="331" spans="1:7">
+      <c r="A331" t="s">
+        <v>272</v>
+      </c>
+      <c r="B331" t="s">
+        <v>51</v>
+      </c>
+      <c r="C331" t="n">
+        <v>10.05</v>
+      </c>
+      <c r="D331" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="E331" t="n">
+        <v>27.34</v>
+      </c>
+    </row>
+    <row r="332" spans="1:7">
+      <c r="A332" t="s">
+        <v>272</v>
+      </c>
+      <c r="B332" t="s">
+        <v>37</v>
+      </c>
+      <c r="C332" t="n">
+        <v>9.880000000000001</v>
+      </c>
+      <c r="D332" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="E332" t="n">
+        <v>25.2</v>
+      </c>
+    </row>
+    <row r="333" spans="1:7">
+      <c r="A333" t="s">
+        <v>272</v>
+      </c>
+      <c r="B333" t="s">
+        <v>38</v>
+      </c>
+      <c r="C333" t="n">
+        <v>10.4</v>
+      </c>
+      <c r="D333" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="E333" t="n">
+        <v>28.11</v>
+      </c>
+    </row>
+    <row r="334" spans="1:7">
+      <c r="A334" t="s">
+        <v>272</v>
+      </c>
+      <c r="B334" t="s">
+        <v>52</v>
+      </c>
+      <c r="C334" t="n">
+        <v>10.35</v>
+      </c>
+      <c r="D334" t="n">
+        <v>7.64</v>
+      </c>
+      <c r="E334" t="n">
+        <v>25.11</v>
+      </c>
+    </row>
+    <row r="335" spans="1:7">
+      <c r="A335" t="s">
+        <v>272</v>
+      </c>
+      <c r="B335" t="s">
+        <v>53</v>
+      </c>
+      <c r="C335" t="n">
+        <v>10.34</v>
+      </c>
+      <c r="D335" t="n">
+        <v>7.3</v>
+      </c>
+      <c r="E335" t="n">
+        <v>34.36</v>
+      </c>
+    </row>
+    <row r="336" spans="1:7">
+      <c r="A336" t="s">
+        <v>272</v>
+      </c>
+      <c r="B336" t="s">
+        <v>54</v>
+      </c>
+      <c r="C336" t="n">
+        <v>10.35</v>
+      </c>
+      <c r="D336" t="n">
+        <v>5.86</v>
+      </c>
+      <c r="E336" t="n">
+        <v>30.63</v>
+      </c>
+    </row>
+    <row r="337" spans="1:7">
+      <c r="A337" t="s">
+        <v>272</v>
+      </c>
+      <c r="B337" t="s">
+        <v>55</v>
+      </c>
+      <c r="C337" t="n">
+        <v>9.779999999999999</v>
+      </c>
+      <c r="D337" t="n">
+        <v>8.91</v>
+      </c>
+      <c r="E337" t="n">
+        <v>27.71</v>
+      </c>
+    </row>
+    <row r="338" spans="1:7">
+      <c r="A338" t="s">
+        <v>272</v>
+      </c>
+      <c r="B338" t="s">
+        <v>56</v>
+      </c>
+      <c r="C338" t="n">
+        <v>10.36</v>
+      </c>
+      <c r="D338" t="n">
+        <v>10.65</v>
+      </c>
+      <c r="E338" t="n">
+        <v>28.39</v>
+      </c>
+    </row>
+    <row r="339" spans="1:7">
+      <c r="A339" t="s">
+        <v>272</v>
+      </c>
+      <c r="B339" t="s">
+        <v>57</v>
+      </c>
+      <c r="C339" t="n">
+        <v>10.37</v>
+      </c>
+      <c r="D339" t="n">
+        <v>10.48</v>
+      </c>
+      <c r="E339" t="n">
+        <v>28.46</v>
+      </c>
+    </row>
+    <row r="340" spans="1:7">
+      <c r="A340" t="s">
+        <v>272</v>
+      </c>
+      <c r="B340" t="s">
+        <v>58</v>
+      </c>
+      <c r="C340" t="n">
+        <v>9.039999999999999</v>
+      </c>
+      <c r="D340" t="n">
+        <v>1.73</v>
+      </c>
+      <c r="E340" t="n">
+        <v>26.42</v>
+      </c>
+    </row>
+    <row r="341" spans="1:7">
+      <c r="A341" t="s">
+        <v>272</v>
+      </c>
+      <c r="B341" t="s">
+        <v>59</v>
+      </c>
+      <c r="C341" t="n">
+        <v>10.36</v>
+      </c>
+      <c r="D341" t="n">
+        <v>10.73</v>
+      </c>
+      <c r="E341" t="n">
+        <v>28.01</v>
+      </c>
+    </row>
+    <row r="342" spans="1:7">
+      <c r="A342" t="s">
+        <v>272</v>
+      </c>
+      <c r="B342" t="s">
+        <v>60</v>
+      </c>
+      <c r="C342" t="n">
+        <v>9.74</v>
+      </c>
+      <c r="D342" t="n">
+        <v>10.46</v>
+      </c>
+      <c r="E342" t="n">
+        <v>27.52</v>
+      </c>
+    </row>
+    <row r="343" spans="1:7">
+      <c r="A343" t="s">
+        <v>272</v>
+      </c>
+      <c r="B343" t="s">
+        <v>61</v>
+      </c>
+      <c r="C343" t="n">
+        <v>10.4</v>
+      </c>
+      <c r="D343" t="n">
+        <v>10.48</v>
+      </c>
+      <c r="E343" t="n">
+        <v>30.42</v>
+      </c>
+    </row>
+    <row r="344" spans="1:7">
+      <c r="A344" t="s">
+        <v>272</v>
+      </c>
+      <c r="B344" t="s">
+        <v>62</v>
+      </c>
+      <c r="C344" t="n">
+        <v>10.24</v>
+      </c>
+      <c r="D344" t="n">
+        <v>10.79</v>
+      </c>
+      <c r="E344" t="n">
+        <v>30.56</v>
+      </c>
+    </row>
+    <row r="345" spans="1:7">
+      <c r="A345" t="s">
+        <v>272</v>
+      </c>
+      <c r="B345" t="s">
+        <v>63</v>
+      </c>
+      <c r="C345" t="n">
+        <v>9.449999999999999</v>
+      </c>
+      <c r="D345" t="n">
+        <v>9.56</v>
+      </c>
+      <c r="E345" t="n">
+        <v>28.13</v>
+      </c>
+    </row>
+    <row r="346" spans="1:7">
+      <c r="A346" t="s">
+        <v>272</v>
+      </c>
+      <c r="B346" t="s">
+        <v>64</v>
+      </c>
+      <c r="C346" t="n">
+        <v>10.35</v>
+      </c>
+      <c r="D346" t="n">
+        <v>6.76</v>
+      </c>
+      <c r="E346" t="n">
+        <v>25.57</v>
+      </c>
+    </row>
+    <row r="347" spans="1:7">
+      <c r="A347" t="s">
+        <v>272</v>
+      </c>
+      <c r="B347" t="s">
+        <v>65</v>
+      </c>
+      <c r="C347" t="n">
+        <v>9.619999999999999</v>
+      </c>
+      <c r="D347" t="n">
+        <v>5.24</v>
+      </c>
+      <c r="E347" t="n">
+        <v>28.77</v>
+      </c>
+    </row>
+    <row r="348" spans="1:7">
+      <c r="A348" t="s">
+        <v>272</v>
+      </c>
+      <c r="B348" t="s">
+        <v>66</v>
+      </c>
+      <c r="C348" t="n">
+        <v>10.12</v>
+      </c>
+      <c r="D348" t="n">
+        <v>5.99</v>
+      </c>
+      <c r="E348" t="n">
+        <v>31.69</v>
+      </c>
+    </row>
+    <row r="349" spans="1:7">
+      <c r="A349" t="s">
+        <v>272</v>
+      </c>
+      <c r="B349" t="s">
+        <v>67</v>
+      </c>
+      <c r="C349" t="n">
+        <v>10.39</v>
+      </c>
+      <c r="D349" t="n">
+        <v>5.16</v>
+      </c>
+      <c r="E349" t="n">
+        <v>30.18</v>
+      </c>
+    </row>
+    <row r="350" spans="1:7">
+      <c r="A350" t="s">
+        <v>272</v>
+      </c>
+      <c r="B350" t="s">
+        <v>68</v>
+      </c>
+      <c r="C350" t="n">
+        <v>10.34</v>
+      </c>
+      <c r="D350" t="n">
+        <v>7.68</v>
+      </c>
+      <c r="E350" t="n">
+        <v>25.22</v>
+      </c>
+    </row>
+    <row r="351" spans="1:7">
+      <c r="A351" t="s">
+        <v>272</v>
+      </c>
+      <c r="B351" t="s">
+        <v>69</v>
+      </c>
+      <c r="C351" t="n">
+        <v>9.94</v>
+      </c>
+      <c r="D351" t="n">
+        <v>7.6</v>
+      </c>
+      <c r="E351" t="n">
+        <v>30.62</v>
+      </c>
+    </row>
+    <row r="352" spans="1:7">
+      <c r="A352" t="s">
+        <v>272</v>
+      </c>
+      <c r="B352" t="s">
+        <v>70</v>
+      </c>
+      <c r="C352" t="n">
+        <v>9.43</v>
+      </c>
+      <c r="D352" t="n">
+        <v>3.53</v>
+      </c>
+      <c r="E352" t="n">
+        <v>28.75</v>
+      </c>
+    </row>
+    <row r="353" spans="1:7">
+      <c r="A353" t="s">
+        <v>272</v>
+      </c>
+      <c r="B353" t="s">
+        <v>71</v>
+      </c>
+      <c r="C353" t="n">
+        <v>10.31</v>
+      </c>
+      <c r="D353" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="E353" t="n">
+        <v>34.78</v>
+      </c>
+    </row>
+    <row r="354" spans="1:7">
+      <c r="A354" t="s">
+        <v>272</v>
+      </c>
+      <c r="B354" t="s">
+        <v>72</v>
+      </c>
+      <c r="C354" t="n">
+        <v>10.28</v>
+      </c>
+      <c r="D354" t="n">
+        <v>4.38</v>
+      </c>
+      <c r="E354" t="n">
+        <v>26.7</v>
+      </c>
+    </row>
+    <row r="355" spans="1:7">
+      <c r="A355" t="s">
+        <v>272</v>
+      </c>
+      <c r="B355" t="s">
+        <v>73</v>
+      </c>
+      <c r="C355" t="n">
+        <v>10.02</v>
+      </c>
+      <c r="D355" t="n">
+        <v>3.82</v>
+      </c>
+      <c r="E355" t="n">
+        <v>40.09</v>
+      </c>
+    </row>
+    <row r="356" spans="1:7">
+      <c r="A356" t="s">
+        <v>272</v>
+      </c>
+      <c r="B356" t="s">
+        <v>74</v>
+      </c>
+      <c r="C356" t="n">
+        <v>9.960000000000001</v>
+      </c>
+      <c r="D356" t="n">
+        <v>2.67</v>
+      </c>
+      <c r="E356" t="n">
+        <v>26.38</v>
+      </c>
+    </row>
+    <row r="357" spans="1:7">
+      <c r="A357" t="s">
+        <v>272</v>
+      </c>
+      <c r="B357" t="s">
+        <v>111</v>
+      </c>
+      <c r="C357" t="n">
+        <v>9.83</v>
+      </c>
+      <c r="D357" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="E357" t="n">
+        <v>38.13</v>
+      </c>
+    </row>
+    <row r="358" spans="1:7">
+      <c r="A358" t="s">
+        <v>272</v>
+      </c>
+      <c r="B358" t="s">
+        <v>113</v>
+      </c>
+      <c r="C358" t="n">
+        <v>10</v>
+      </c>
+      <c r="D358" t="n">
+        <v>1.16</v>
+      </c>
+      <c r="E358" t="n">
+        <v>33.02</v>
+      </c>
+    </row>
+    <row r="359" spans="1:7">
+      <c r="A359" t="s">
+        <v>272</v>
+      </c>
+      <c r="B359" t="s">
+        <v>39</v>
+      </c>
+      <c r="C359" t="n">
+        <v>7.86</v>
+      </c>
+      <c r="D359" t="n">
+        <v>1.63</v>
+      </c>
+      <c r="E359" t="n">
+        <v>50.26</v>
+      </c>
+    </row>
+    <row r="360" spans="1:7">
+      <c r="A360" t="s">
+        <v>272</v>
+      </c>
+      <c r="B360" t="s">
+        <v>40</v>
+      </c>
+      <c r="C360" t="n">
+        <v>9.18</v>
+      </c>
+      <c r="D360" t="n">
+        <v>1.71</v>
+      </c>
+      <c r="E360" t="n">
+        <v>37.93</v>
+      </c>
+    </row>
+    <row r="361" spans="1:7">
+      <c r="A361" t="s">
+        <v>272</v>
+      </c>
+      <c r="B361" t="s">
+        <v>11</v>
+      </c>
+      <c r="C361" t="n">
+        <v>10.02</v>
+      </c>
+      <c r="D361" t="n">
+        <v>2.26</v>
+      </c>
+      <c r="E361" t="n">
+        <v>36.2</v>
+      </c>
+    </row>
+    <row r="362" spans="1:7">
+      <c r="A362" t="s">
+        <v>272</v>
+      </c>
+      <c r="B362" t="s">
+        <v>17</v>
+      </c>
+      <c r="C362" t="n">
+        <v>9.75</v>
+      </c>
+      <c r="D362" t="n">
+        <v>2.11</v>
+      </c>
+      <c r="E362" t="n">
+        <v>29.61</v>
+      </c>
+    </row>
+    <row r="363" spans="1:7">
+      <c r="A363" t="s">
+        <v>272</v>
+      </c>
+      <c r="B363" t="s">
+        <v>23</v>
+      </c>
+      <c r="C363" t="n">
+        <v>10.01</v>
+      </c>
+      <c r="D363" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="E363" t="n">
+        <v>36.34</v>
+      </c>
+    </row>
+    <row r="364" spans="1:7">
+      <c r="A364" t="s">
+        <v>272</v>
+      </c>
+      <c r="B364" t="s">
+        <v>28</v>
+      </c>
+      <c r="C364" t="n">
+        <v>10.21</v>
+      </c>
+      <c r="D364" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E364" t="n">
+        <v>36.78</v>
+      </c>
+    </row>
+    <row r="365" spans="1:7">
+      <c r="A365" t="s">
+        <v>272</v>
+      </c>
+      <c r="B365" t="s">
+        <v>41</v>
+      </c>
+      <c r="C365" t="n">
+        <v>10.3</v>
+      </c>
+      <c r="D365" t="n">
+        <v>3.42</v>
+      </c>
+      <c r="E365" t="n">
+        <v>34.67</v>
+      </c>
+    </row>
+    <row r="366" spans="1:7">
+      <c r="A366" t="s">
+        <v>272</v>
+      </c>
+      <c r="B366" t="s">
+        <v>42</v>
+      </c>
+      <c r="C366" t="n">
+        <v>10.27</v>
+      </c>
+      <c r="D366" t="n">
+        <v>3.37</v>
+      </c>
+      <c r="E366" t="n">
+        <v>28.54</v>
+      </c>
+    </row>
+    <row r="367" spans="1:7">
+      <c r="A367" t="s">
+        <v>272</v>
+      </c>
+      <c r="B367" t="s">
+        <v>43</v>
+      </c>
+      <c r="C367" t="n">
+        <v>10.37</v>
+      </c>
+      <c r="D367" t="n">
+        <v>3.73</v>
+      </c>
+      <c r="E367" t="n">
+        <v>35.63</v>
+      </c>
+    </row>
+    <row r="368" spans="1:7">
+      <c r="A368" t="s">
+        <v>272</v>
+      </c>
+      <c r="B368" t="s">
+        <v>44</v>
+      </c>
+      <c r="C368" t="n">
+        <v>9.07</v>
+      </c>
+      <c r="D368" t="n">
+        <v>1.48</v>
+      </c>
+      <c r="E368" t="n">
+        <v>46.33</v>
+      </c>
+    </row>
+    <row r="369" spans="1:7">
+      <c r="A369" t="s">
+        <v>272</v>
+      </c>
+      <c r="B369" t="s">
+        <v>45</v>
+      </c>
+      <c r="C369" t="n">
+        <v>9.24</v>
+      </c>
+      <c r="D369" t="n">
+        <v>2.59</v>
+      </c>
+      <c r="E369" t="n">
+        <v>32.24</v>
+      </c>
+    </row>
+    <row r="370" spans="1:7">
+      <c r="A370" t="s">
+        <v>272</v>
+      </c>
+      <c r="B370" t="s">
+        <v>46</v>
+      </c>
+      <c r="C370" t="n">
+        <v>9.83</v>
+      </c>
+      <c r="D370" t="n">
+        <v>1.18</v>
+      </c>
+      <c r="E370" t="n">
+        <v>45.37</v>
+      </c>
+    </row>
+    <row r="371" spans="1:7">
+      <c r="A371" t="s">
+        <v>272</v>
+      </c>
+      <c r="B371" t="s">
+        <v>47</v>
+      </c>
+      <c r="C371" t="n">
+        <v>9.48</v>
+      </c>
+      <c r="D371" t="n">
+        <v>2.04</v>
+      </c>
+      <c r="E371" t="n">
+        <v>45.72</v>
+      </c>
+    </row>
+    <row r="372" spans="1:7">
+      <c r="A372" t="s">
+        <v>272</v>
+      </c>
+      <c r="B372" t="s">
+        <v>48</v>
+      </c>
+      <c r="C372" t="n">
+        <v>8.75</v>
+      </c>
+      <c r="D372" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E372" t="n">
+        <v>56.85</v>
+      </c>
+    </row>
+    <row r="373" spans="1:7">
+      <c r="A373" t="s">
+        <v>272</v>
+      </c>
+      <c r="B373" t="s">
+        <v>31</v>
+      </c>
+      <c r="C373" t="n">
+        <v>8.58</v>
+      </c>
+      <c r="D373" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="E373" t="n">
+        <v>47.7</v>
+      </c>
+    </row>
+    <row r="374" spans="1:7">
+      <c r="A374" t="s">
+        <v>272</v>
+      </c>
+      <c r="B374" t="s">
+        <v>32</v>
+      </c>
+      <c r="C374" t="n">
+        <v>9.710000000000001</v>
+      </c>
+      <c r="D374" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="E374" t="n">
+        <v>49.61</v>
+      </c>
+    </row>
+    <row r="375" spans="1:7">
+      <c r="A375" t="s">
+        <v>272</v>
+      </c>
+      <c r="B375" t="s">
+        <v>33</v>
+      </c>
+      <c r="C375" t="n">
+        <v>2.48</v>
+      </c>
+      <c r="D375" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E375" t="n">
+        <v>434.15</v>
+      </c>
+    </row>
+    <row r="376" spans="1:7">
+      <c r="A376" t="s">
+        <v>272</v>
+      </c>
+      <c r="B376" t="s">
+        <v>34</v>
+      </c>
+      <c r="C376" t="n">
+        <v>9.460000000000001</v>
+      </c>
+      <c r="D376" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="E376" t="n">
+        <v>44.77</v>
+      </c>
+    </row>
+    <row r="377" spans="1:7">
+      <c r="A377" t="s">
+        <v>272</v>
+      </c>
+      <c r="B377" t="s">
+        <v>35</v>
+      </c>
+      <c r="C377" t="n">
+        <v>9.23</v>
+      </c>
+      <c r="D377" t="n">
+        <v>3.21</v>
+      </c>
+      <c r="E377" t="n">
+        <v>31.51</v>
+      </c>
+    </row>
+    <row r="378" spans="1:7">
+      <c r="A378" t="s">
+        <v>273</v>
+      </c>
+      <c r="B378" t="s">
+        <v>50</v>
+      </c>
+      <c r="C378" t="n">
+        <v>8.32</v>
+      </c>
+      <c r="D378" t="n">
+        <v>4.54</v>
+      </c>
+      <c r="E378" t="n">
+        <v>63.05</v>
+      </c>
+    </row>
+    <row r="379" spans="1:7">
+      <c r="A379" t="s">
+        <v>273</v>
+      </c>
+      <c r="B379" t="s">
+        <v>51</v>
+      </c>
+      <c r="C379" t="n">
+        <v>9.630000000000001</v>
+      </c>
+      <c r="D379" t="n">
+        <v>4.16</v>
+      </c>
+      <c r="E379" t="n">
+        <v>34.81</v>
+      </c>
+    </row>
+    <row r="380" spans="1:7">
+      <c r="A380" t="s">
+        <v>273</v>
+      </c>
+      <c r="B380" t="s">
+        <v>37</v>
+      </c>
+      <c r="C380" t="n">
+        <v>10.38</v>
+      </c>
+      <c r="D380" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="E380" t="n">
+        <v>28.31</v>
+      </c>
+    </row>
+    <row r="381" spans="1:7">
+      <c r="A381" t="s">
+        <v>273</v>
+      </c>
+      <c r="B381" t="s">
+        <v>38</v>
+      </c>
+      <c r="C381" t="n">
+        <v>8.869999999999999</v>
+      </c>
+      <c r="D381" t="n">
+        <v>5.87</v>
+      </c>
+      <c r="E381" t="n">
+        <v>29.72</v>
+      </c>
+    </row>
+    <row r="382" spans="1:7">
+      <c r="A382" t="s">
+        <v>273</v>
+      </c>
+      <c r="B382" t="s">
+        <v>52</v>
+      </c>
+      <c r="C382" t="n">
+        <v>10.35</v>
+      </c>
+      <c r="D382" t="n">
+        <v>5.31</v>
+      </c>
+      <c r="E382" t="n">
+        <v>25.53</v>
+      </c>
+    </row>
+    <row r="383" spans="1:7">
+      <c r="A383" t="s">
+        <v>273</v>
+      </c>
+      <c r="B383" t="s">
+        <v>53</v>
+      </c>
+      <c r="C383" t="n">
+        <v>10.39</v>
+      </c>
+      <c r="D383" t="n">
+        <v>9.98</v>
+      </c>
+      <c r="E383" t="n">
+        <v>29.73</v>
+      </c>
+    </row>
+    <row r="384" spans="1:7">
+      <c r="A384" t="s">
+        <v>273</v>
+      </c>
+      <c r="B384" t="s">
+        <v>54</v>
+      </c>
+      <c r="C384" t="n">
+        <v>9.59</v>
+      </c>
+      <c r="D384" t="n">
+        <v>8.85</v>
+      </c>
+      <c r="E384" t="n">
+        <v>29.72</v>
+      </c>
+    </row>
+    <row r="385" spans="1:7">
+      <c r="A385" t="s">
+        <v>273</v>
+      </c>
+      <c r="B385" t="s">
+        <v>55</v>
+      </c>
+      <c r="C385" t="n">
+        <v>10.35</v>
+      </c>
+      <c r="D385" t="n">
+        <v>10.22</v>
+      </c>
+      <c r="E385" t="n">
+        <v>28.94</v>
+      </c>
+    </row>
+    <row r="386" spans="1:7">
+      <c r="A386" t="s">
+        <v>273</v>
+      </c>
+      <c r="B386" t="s">
+        <v>56</v>
+      </c>
+      <c r="C386" t="n">
+        <v>6.65</v>
+      </c>
+      <c r="D386" t="n">
+        <v>10.46</v>
+      </c>
+      <c r="E386" t="n">
+        <v>34.2</v>
+      </c>
+    </row>
+    <row r="387" spans="1:7">
+      <c r="A387" t="s">
+        <v>273</v>
+      </c>
+      <c r="B387" t="s">
+        <v>57</v>
+      </c>
+      <c r="C387" t="n">
+        <v>10.19</v>
+      </c>
+      <c r="D387" t="n">
+        <v>10.04</v>
+      </c>
+      <c r="E387" t="n">
+        <v>32.24</v>
+      </c>
+    </row>
+    <row r="388" spans="1:7">
+      <c r="A388" t="s">
+        <v>273</v>
+      </c>
+      <c r="B388" t="s">
+        <v>58</v>
+      </c>
+      <c r="C388" t="n">
+        <v>8.65</v>
+      </c>
+      <c r="D388" t="n">
+        <v>10.78</v>
+      </c>
+      <c r="E388" t="n">
+        <v>26.34</v>
+      </c>
+    </row>
+    <row r="389" spans="1:7">
+      <c r="A389" t="s">
+        <v>273</v>
+      </c>
+      <c r="B389" t="s">
+        <v>59</v>
+      </c>
+      <c r="C389" t="n">
+        <v>10.38</v>
+      </c>
+      <c r="D389" t="n">
+        <v>10.74</v>
+      </c>
+      <c r="E389" t="n">
+        <v>31.26</v>
+      </c>
+    </row>
+    <row r="390" spans="1:7">
+      <c r="A390" t="s">
+        <v>273</v>
+      </c>
+      <c r="B390" t="s">
+        <v>60</v>
+      </c>
+      <c r="C390" t="n">
+        <v>10.38</v>
+      </c>
+      <c r="D390" t="n">
+        <v>6.34</v>
+      </c>
+      <c r="E390" t="n">
+        <v>26.36</v>
+      </c>
+    </row>
+    <row r="391" spans="1:7">
+      <c r="A391" t="s">
+        <v>273</v>
+      </c>
+      <c r="B391" t="s">
+        <v>61</v>
+      </c>
+      <c r="C391" t="n">
+        <v>10.34</v>
+      </c>
+      <c r="D391" t="n">
+        <v>10.82</v>
+      </c>
+      <c r="E391" t="n">
+        <v>30.92</v>
+      </c>
+    </row>
+    <row r="392" spans="1:7">
+      <c r="A392" t="s">
+        <v>273</v>
+      </c>
+      <c r="B392" t="s">
+        <v>62</v>
+      </c>
+      <c r="C392" t="n">
+        <v>10.37</v>
+      </c>
+      <c r="D392" t="n">
+        <v>10.52</v>
+      </c>
+      <c r="E392" t="n">
+        <v>25.06</v>
+      </c>
+    </row>
+    <row r="393" spans="1:7">
+      <c r="A393" t="s">
+        <v>273</v>
+      </c>
+      <c r="B393" t="s">
+        <v>63</v>
+      </c>
+      <c r="C393" t="n">
+        <v>9.960000000000001</v>
+      </c>
+      <c r="D393" t="n">
+        <v>4.53</v>
+      </c>
+      <c r="E393" t="n">
+        <v>37.97</v>
+      </c>
+    </row>
+    <row r="394" spans="1:7">
+      <c r="A394" t="s">
+        <v>273</v>
+      </c>
+      <c r="B394" t="s">
+        <v>64</v>
+      </c>
+      <c r="C394" t="n">
+        <v>10.36</v>
+      </c>
+      <c r="D394" t="n">
+        <v>5.66</v>
+      </c>
+      <c r="E394" t="n">
+        <v>35.05</v>
+      </c>
+    </row>
+    <row r="395" spans="1:7">
+      <c r="A395" t="s">
+        <v>273</v>
+      </c>
+      <c r="B395" t="s">
+        <v>65</v>
+      </c>
+      <c r="C395" t="n">
+        <v>9.94</v>
+      </c>
+      <c r="D395" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E395" t="n">
+        <v>29.05</v>
+      </c>
+    </row>
+    <row r="396" spans="1:7">
+      <c r="A396" t="s">
+        <v>273</v>
+      </c>
+      <c r="B396" t="s">
+        <v>66</v>
+      </c>
+      <c r="C396" t="n">
+        <v>10.31</v>
+      </c>
+      <c r="D396" t="n">
+        <v>3.81</v>
+      </c>
+      <c r="E396" t="n">
+        <v>25.16</v>
+      </c>
+    </row>
+    <row r="397" spans="1:7">
+      <c r="A397" t="s">
+        <v>273</v>
+      </c>
+      <c r="B397" t="s">
+        <v>67</v>
+      </c>
+      <c r="C397" t="n">
+        <v>10.31</v>
+      </c>
+      <c r="D397" t="n">
+        <v>3.46</v>
+      </c>
+      <c r="E397" t="n">
+        <v>28.93</v>
+      </c>
+    </row>
+    <row r="398" spans="1:7">
+      <c r="A398" t="s">
+        <v>273</v>
+      </c>
+      <c r="B398" t="s">
+        <v>68</v>
+      </c>
+      <c r="C398" t="n">
+        <v>9.699999999999999</v>
+      </c>
+      <c r="D398" t="n">
+        <v>9.609999999999999</v>
+      </c>
+      <c r="E398" t="n">
+        <v>28.85</v>
+      </c>
+    </row>
+    <row r="399" spans="1:7">
+      <c r="A399" t="s">
+        <v>273</v>
+      </c>
+      <c r="B399" t="s">
+        <v>69</v>
+      </c>
+      <c r="C399" t="n">
+        <v>10.37</v>
+      </c>
+      <c r="D399" t="n">
+        <v>5.61</v>
+      </c>
+      <c r="E399" t="n">
+        <v>28.84</v>
+      </c>
+    </row>
+    <row r="400" spans="1:7">
+      <c r="A400" t="s">
+        <v>273</v>
+      </c>
+      <c r="B400" t="s">
+        <v>70</v>
+      </c>
+      <c r="C400" t="n">
+        <v>9.199999999999999</v>
+      </c>
+      <c r="D400" t="n">
+        <v>3.32</v>
+      </c>
+      <c r="E400" t="n">
+        <v>25.65</v>
+      </c>
+    </row>
+    <row r="401" spans="1:7">
+      <c r="A401" t="s">
+        <v>273</v>
+      </c>
+      <c r="B401" t="s">
+        <v>71</v>
+      </c>
+      <c r="C401" t="n">
+        <v>10.4</v>
+      </c>
+      <c r="D401" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="E401" t="n">
+        <v>34.31</v>
+      </c>
+    </row>
+    <row r="402" spans="1:7">
+      <c r="A402" t="s">
+        <v>273</v>
+      </c>
+      <c r="B402" t="s">
+        <v>72</v>
+      </c>
+      <c r="C402" t="n">
+        <v>9.1</v>
+      </c>
+      <c r="D402" t="n">
+        <v>4.07</v>
+      </c>
+      <c r="E402" t="n">
+        <v>29.55</v>
       </c>
     </row>
     <row customHeight="1" ht="12.8" r="1048576" s="6" spans="1:7"/>

</xml_diff>